<commit_message>
INTYGFV-12747: Lagt in ny statistik från FK för 2017
</commit_message>
<xml_diff>
--- a/web/src/main/resources/nationellstatistik.xlsx
+++ b/web/src/main/resources/nationellstatistik.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10309"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10209"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/christian/Development/inera/intyg/srs/src/main/resources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/christian/Development/inera/intyg/srs/web/src/main/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59077915-65B2-D84D-9139-379716E76EB0}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{996D48BB-4016-A049-AD18-5C9943E42BE4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38440" yWindow="25200" windowWidth="28800" windowHeight="11740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10440" yWindow="24940" windowWidth="37200" windowHeight="15660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Antal fall" sheetId="1" r:id="rId1"/>
     <sheet name="Antal personer" sheetId="2" r:id="rId2"/>
+    <sheet name="Antal fall 2015" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -24,7 +25,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -32,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="41">
   <si>
     <t>F31</t>
   </si>
@@ -146,6 +149,15 @@
   </si>
   <si>
     <t>Antal unika personer per diagnos för antal startade sjukfall (&gt;14 dagar) under 2015</t>
+  </si>
+  <si>
+    <t>&gt;=365 dagar</t>
+  </si>
+  <si>
+    <t>180-364 dagar</t>
+  </si>
+  <si>
+    <t>Diagnosfördelning för antal startade sjukfall (&gt;14 dagar) under 2017</t>
   </si>
 </sst>
 </file>
@@ -467,7 +479,1013 @@
   <dimension ref="A1:AB10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="21.83203125" customWidth="1"/>
+    <col min="2" max="2" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="16" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="19" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="21" max="27" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="10.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="B3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="B4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F4" t="s">
+        <v>4</v>
+      </c>
+      <c r="G4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H4" t="s">
+        <v>6</v>
+      </c>
+      <c r="I4" t="s">
+        <v>8</v>
+      </c>
+      <c r="J4" t="s">
+        <v>9</v>
+      </c>
+      <c r="K4" t="s">
+        <v>11</v>
+      </c>
+      <c r="L4" t="s">
+        <v>12</v>
+      </c>
+      <c r="M4" t="s">
+        <v>13</v>
+      </c>
+      <c r="N4" t="s">
+        <v>14</v>
+      </c>
+      <c r="O4" t="s">
+        <v>15</v>
+      </c>
+      <c r="P4" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>17</v>
+      </c>
+      <c r="R4" t="s">
+        <v>18</v>
+      </c>
+      <c r="S4" t="s">
+        <v>20</v>
+      </c>
+      <c r="T4" t="s">
+        <v>21</v>
+      </c>
+      <c r="U4" t="s">
+        <v>22</v>
+      </c>
+      <c r="V4" t="s">
+        <v>23</v>
+      </c>
+      <c r="W4" t="s">
+        <v>24</v>
+      </c>
+      <c r="X4" t="s">
+        <v>25</v>
+      </c>
+      <c r="Y4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B5">
+        <v>911</v>
+      </c>
+      <c r="C5">
+        <v>3559</v>
+      </c>
+      <c r="D5">
+        <v>1824</v>
+      </c>
+      <c r="E5">
+        <v>2587</v>
+      </c>
+      <c r="F5">
+        <v>8288</v>
+      </c>
+      <c r="G5">
+        <v>78</v>
+      </c>
+      <c r="H5">
+        <v>572</v>
+      </c>
+      <c r="I5">
+        <v>139</v>
+      </c>
+      <c r="J5">
+        <v>203</v>
+      </c>
+      <c r="K5">
+        <v>111</v>
+      </c>
+      <c r="L5">
+        <v>39</v>
+      </c>
+      <c r="M5">
+        <v>338</v>
+      </c>
+      <c r="N5">
+        <v>225</v>
+      </c>
+      <c r="O5">
+        <v>1235</v>
+      </c>
+      <c r="P5">
+        <v>304</v>
+      </c>
+      <c r="Q5">
+        <v>77</v>
+      </c>
+      <c r="R5">
+        <v>564</v>
+      </c>
+      <c r="S5">
+        <v>282</v>
+      </c>
+      <c r="T5">
+        <v>242</v>
+      </c>
+      <c r="U5">
+        <v>61</v>
+      </c>
+      <c r="V5">
+        <v>26</v>
+      </c>
+      <c r="W5">
+        <v>99</v>
+      </c>
+      <c r="X5">
+        <v>58</v>
+      </c>
+      <c r="Y5">
+        <v>21822</v>
+      </c>
+      <c r="Z5" s="1"/>
+      <c r="AA5" s="1"/>
+      <c r="AB5" s="1"/>
+    </row>
+    <row r="6" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B6">
+        <v>358</v>
+      </c>
+      <c r="C6">
+        <v>3215</v>
+      </c>
+      <c r="D6">
+        <v>936</v>
+      </c>
+      <c r="E6">
+        <v>3695</v>
+      </c>
+      <c r="F6">
+        <v>13432</v>
+      </c>
+      <c r="G6">
+        <v>1598</v>
+      </c>
+      <c r="H6">
+        <v>84</v>
+      </c>
+      <c r="I6">
+        <v>260</v>
+      </c>
+      <c r="J6">
+        <v>717</v>
+      </c>
+      <c r="K6">
+        <v>409</v>
+      </c>
+      <c r="L6">
+        <v>1313</v>
+      </c>
+      <c r="M6">
+        <v>826</v>
+      </c>
+      <c r="N6">
+        <v>574</v>
+      </c>
+      <c r="O6">
+        <v>10778</v>
+      </c>
+      <c r="P6">
+        <v>1902</v>
+      </c>
+      <c r="Q6">
+        <v>1330</v>
+      </c>
+      <c r="R6">
+        <v>3741</v>
+      </c>
+      <c r="S6">
+        <v>928</v>
+      </c>
+      <c r="T6">
+        <v>927</v>
+      </c>
+      <c r="U6">
+        <v>1036</v>
+      </c>
+      <c r="V6">
+        <v>1363</v>
+      </c>
+      <c r="W6">
+        <v>620</v>
+      </c>
+      <c r="X6">
+        <v>1364</v>
+      </c>
+      <c r="Y6">
+        <v>51406</v>
+      </c>
+      <c r="Z6" s="1"/>
+      <c r="AA6" s="1"/>
+      <c r="AB6" s="1"/>
+    </row>
+    <row r="7" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>39</v>
+      </c>
+      <c r="B7">
+        <v>540</v>
+      </c>
+      <c r="C7">
+        <v>4301</v>
+      </c>
+      <c r="D7">
+        <v>1611</v>
+      </c>
+      <c r="E7">
+        <v>3010</v>
+      </c>
+      <c r="F7">
+        <v>12435</v>
+      </c>
+      <c r="G7">
+        <v>268</v>
+      </c>
+      <c r="H7">
+        <v>327</v>
+      </c>
+      <c r="I7">
+        <v>606</v>
+      </c>
+      <c r="J7">
+        <v>907</v>
+      </c>
+      <c r="K7">
+        <v>382</v>
+      </c>
+      <c r="L7">
+        <v>215</v>
+      </c>
+      <c r="M7">
+        <v>670</v>
+      </c>
+      <c r="N7">
+        <v>369</v>
+      </c>
+      <c r="O7">
+        <v>2756</v>
+      </c>
+      <c r="P7">
+        <v>1172</v>
+      </c>
+      <c r="Q7">
+        <v>332</v>
+      </c>
+      <c r="R7">
+        <v>1191</v>
+      </c>
+      <c r="S7">
+        <v>312</v>
+      </c>
+      <c r="T7">
+        <v>254</v>
+      </c>
+      <c r="U7">
+        <v>286</v>
+      </c>
+      <c r="V7">
+        <v>145</v>
+      </c>
+      <c r="W7">
+        <v>496</v>
+      </c>
+      <c r="X7">
+        <v>432</v>
+      </c>
+      <c r="Y7">
+        <v>33017</v>
+      </c>
+      <c r="Z7" s="1"/>
+      <c r="AA7" s="1"/>
+      <c r="AB7" s="1"/>
+    </row>
+    <row r="8" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>29</v>
+      </c>
+      <c r="B8">
+        <v>1079</v>
+      </c>
+      <c r="C8">
+        <v>9108</v>
+      </c>
+      <c r="D8">
+        <v>2867</v>
+      </c>
+      <c r="E8">
+        <v>7910</v>
+      </c>
+      <c r="F8">
+        <v>24062</v>
+      </c>
+      <c r="G8">
+        <v>4818</v>
+      </c>
+      <c r="H8">
+        <v>325</v>
+      </c>
+      <c r="I8">
+        <v>1649</v>
+      </c>
+      <c r="J8">
+        <v>1942</v>
+      </c>
+      <c r="K8">
+        <v>1033</v>
+      </c>
+      <c r="L8">
+        <v>1823</v>
+      </c>
+      <c r="M8">
+        <v>1900</v>
+      </c>
+      <c r="N8">
+        <v>859</v>
+      </c>
+      <c r="O8">
+        <v>10764</v>
+      </c>
+      <c r="P8">
+        <v>3682</v>
+      </c>
+      <c r="Q8">
+        <v>1561</v>
+      </c>
+      <c r="R8">
+        <v>3768</v>
+      </c>
+      <c r="S8">
+        <v>873</v>
+      </c>
+      <c r="T8">
+        <v>939</v>
+      </c>
+      <c r="U8">
+        <v>4122</v>
+      </c>
+      <c r="V8">
+        <v>3286</v>
+      </c>
+      <c r="W8">
+        <v>3451</v>
+      </c>
+      <c r="X8">
+        <v>2248</v>
+      </c>
+      <c r="Y8">
+        <v>94069</v>
+      </c>
+      <c r="Z8" s="1"/>
+      <c r="AA8" s="1"/>
+      <c r="AB8" s="1"/>
+    </row>
+    <row r="9" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>31</v>
+      </c>
+      <c r="B9">
+        <v>679</v>
+      </c>
+      <c r="C9">
+        <v>5433</v>
+      </c>
+      <c r="D9">
+        <v>1832</v>
+      </c>
+      <c r="E9">
+        <v>3968</v>
+      </c>
+      <c r="F9">
+        <v>13023</v>
+      </c>
+      <c r="G9">
+        <v>526</v>
+      </c>
+      <c r="H9">
+        <v>289</v>
+      </c>
+      <c r="I9">
+        <v>1553</v>
+      </c>
+      <c r="J9">
+        <v>2060</v>
+      </c>
+      <c r="K9">
+        <v>607</v>
+      </c>
+      <c r="L9">
+        <v>686</v>
+      </c>
+      <c r="M9">
+        <v>909</v>
+      </c>
+      <c r="N9">
+        <v>391</v>
+      </c>
+      <c r="O9">
+        <v>3795</v>
+      </c>
+      <c r="P9">
+        <v>1721</v>
+      </c>
+      <c r="Q9">
+        <v>509</v>
+      </c>
+      <c r="R9">
+        <v>1408</v>
+      </c>
+      <c r="S9">
+        <v>322</v>
+      </c>
+      <c r="T9">
+        <v>363</v>
+      </c>
+      <c r="U9">
+        <v>901</v>
+      </c>
+      <c r="V9">
+        <v>556</v>
+      </c>
+      <c r="W9">
+        <v>1420</v>
+      </c>
+      <c r="X9">
+        <v>886</v>
+      </c>
+      <c r="Y9">
+        <v>43837</v>
+      </c>
+      <c r="Z9" s="1"/>
+      <c r="AA9" s="1"/>
+      <c r="AB9" s="1"/>
+    </row>
+    <row r="10" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10">
+        <v>3567</v>
+      </c>
+      <c r="C10">
+        <v>25616</v>
+      </c>
+      <c r="D10">
+        <v>9070</v>
+      </c>
+      <c r="E10">
+        <v>21170</v>
+      </c>
+      <c r="F10">
+        <v>71240</v>
+      </c>
+      <c r="G10">
+        <v>7288</v>
+      </c>
+      <c r="H10">
+        <v>1597</v>
+      </c>
+      <c r="I10">
+        <v>4207</v>
+      </c>
+      <c r="J10">
+        <v>5829</v>
+      </c>
+      <c r="K10">
+        <v>2542</v>
+      </c>
+      <c r="L10">
+        <v>4076</v>
+      </c>
+      <c r="M10">
+        <v>4643</v>
+      </c>
+      <c r="N10">
+        <v>2418</v>
+      </c>
+      <c r="O10">
+        <v>29328</v>
+      </c>
+      <c r="P10">
+        <v>8781</v>
+      </c>
+      <c r="Q10">
+        <v>3809</v>
+      </c>
+      <c r="R10">
+        <v>10672</v>
+      </c>
+      <c r="S10">
+        <v>2717</v>
+      </c>
+      <c r="T10">
+        <v>2725</v>
+      </c>
+      <c r="U10">
+        <v>6406</v>
+      </c>
+      <c r="V10">
+        <v>5376</v>
+      </c>
+      <c r="W10">
+        <v>6086</v>
+      </c>
+      <c r="X10">
+        <v>4988</v>
+      </c>
+      <c r="Y10">
+        <v>244151</v>
+      </c>
+      <c r="Z10" s="1"/>
+      <c r="AA10" s="1"/>
+      <c r="AB10" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:D32"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J14" sqref="J14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5">
+        <v>2313</v>
+      </c>
+      <c r="C5">
+        <v>1155</v>
+      </c>
+      <c r="D5">
+        <v>3468</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6">
+        <v>19784</v>
+      </c>
+      <c r="C6">
+        <v>9427</v>
+      </c>
+      <c r="D6">
+        <v>29211</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7">
+        <v>5635</v>
+      </c>
+      <c r="C7">
+        <v>2492</v>
+      </c>
+      <c r="D7">
+        <v>8127</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8">
+        <v>12773</v>
+      </c>
+      <c r="C8">
+        <v>5990</v>
+      </c>
+      <c r="D8">
+        <v>18763</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9">
+        <v>49718</v>
+      </c>
+      <c r="C9">
+        <v>15844</v>
+      </c>
+      <c r="D9">
+        <v>65562</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10">
+        <v>4637</v>
+      </c>
+      <c r="C10">
+        <v>2036</v>
+      </c>
+      <c r="D10">
+        <v>6673</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11">
+        <v>579</v>
+      </c>
+      <c r="C11">
+        <v>1071</v>
+      </c>
+      <c r="D11">
+        <v>1650</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>7</v>
+      </c>
+      <c r="B12">
+        <v>173</v>
+      </c>
+      <c r="C12">
+        <v>48</v>
+      </c>
+      <c r="D12">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>8</v>
+      </c>
+      <c r="B13">
+        <v>1842</v>
+      </c>
+      <c r="C13">
+        <v>1929</v>
+      </c>
+      <c r="D13">
+        <v>3771</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>9</v>
+      </c>
+      <c r="B14">
+        <v>2819</v>
+      </c>
+      <c r="C14">
+        <v>2388</v>
+      </c>
+      <c r="D14">
+        <v>5207</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>10</v>
+      </c>
+      <c r="B15">
+        <v>708</v>
+      </c>
+      <c r="C15">
+        <v>193</v>
+      </c>
+      <c r="D15">
+        <v>901</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>11</v>
+      </c>
+      <c r="B16">
+        <v>1358</v>
+      </c>
+      <c r="C16">
+        <v>1294</v>
+      </c>
+      <c r="D16">
+        <v>2652</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>12</v>
+      </c>
+      <c r="B17">
+        <v>1820</v>
+      </c>
+      <c r="C17">
+        <v>2570</v>
+      </c>
+      <c r="D17">
+        <v>4390</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>13</v>
+      </c>
+      <c r="B18">
+        <v>2284</v>
+      </c>
+      <c r="C18">
+        <v>2312</v>
+      </c>
+      <c r="D18">
+        <v>4596</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>14</v>
+      </c>
+      <c r="B19">
+        <v>1942</v>
+      </c>
+      <c r="C19">
+        <v>1079</v>
+      </c>
+      <c r="D19">
+        <v>3021</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>15</v>
+      </c>
+      <c r="B20">
+        <v>16975</v>
+      </c>
+      <c r="C20">
+        <v>13606</v>
+      </c>
+      <c r="D20">
+        <v>30581</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>16</v>
+      </c>
+      <c r="B21">
+        <v>4912</v>
+      </c>
+      <c r="C21">
+        <v>4412</v>
+      </c>
+      <c r="D21">
+        <v>9324</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>17</v>
+      </c>
+      <c r="B22">
+        <v>2562</v>
+      </c>
+      <c r="C22">
+        <v>1754</v>
+      </c>
+      <c r="D22">
+        <v>4316</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>18</v>
+      </c>
+      <c r="B23">
+        <v>7817</v>
+      </c>
+      <c r="C23">
+        <v>3731</v>
+      </c>
+      <c r="D23">
+        <v>11548</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>19</v>
+      </c>
+      <c r="B24">
+        <v>1032</v>
+      </c>
+      <c r="C24">
+        <v>465</v>
+      </c>
+      <c r="D24">
+        <v>1497</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>20</v>
+      </c>
+      <c r="B25">
+        <v>1860</v>
+      </c>
+      <c r="C25">
+        <v>945</v>
+      </c>
+      <c r="D25">
+        <v>2805</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>21</v>
+      </c>
+      <c r="B26">
+        <v>2270</v>
+      </c>
+      <c r="C26">
+        <v>756</v>
+      </c>
+      <c r="D26">
+        <v>3026</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>22</v>
+      </c>
+      <c r="B27">
+        <v>4007</v>
+      </c>
+      <c r="C27">
+        <v>1945</v>
+      </c>
+      <c r="D27">
+        <v>5952</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>23</v>
+      </c>
+      <c r="B28">
+        <v>1685</v>
+      </c>
+      <c r="C28">
+        <v>3530</v>
+      </c>
+      <c r="D28">
+        <v>5215</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>24</v>
+      </c>
+      <c r="B29">
+        <v>3025</v>
+      </c>
+      <c r="C29">
+        <v>2825</v>
+      </c>
+      <c r="D29">
+        <v>5850</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>25</v>
+      </c>
+      <c r="B30">
+        <v>1958</v>
+      </c>
+      <c r="C30">
+        <v>2556</v>
+      </c>
+      <c r="D30">
+        <v>4514</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>26</v>
+      </c>
+      <c r="B32">
+        <v>156488</v>
+      </c>
+      <c r="C32">
+        <v>86353</v>
+      </c>
+      <c r="D32">
+        <v>242841</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE0ABBB5-F7D0-5F4C-BF5A-F173E972FF30}">
+  <dimension ref="A1:AB10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1102,413 +2120,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:D32"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B4" t="s">
-        <v>34</v>
-      </c>
-      <c r="C4" t="s">
-        <v>35</v>
-      </c>
-      <c r="D4" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B5">
-        <v>2313</v>
-      </c>
-      <c r="C5">
-        <v>1155</v>
-      </c>
-      <c r="D5">
-        <v>3468</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>1</v>
-      </c>
-      <c r="B6">
-        <v>19784</v>
-      </c>
-      <c r="C6">
-        <v>9427</v>
-      </c>
-      <c r="D6">
-        <v>29211</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>2</v>
-      </c>
-      <c r="B7">
-        <v>5635</v>
-      </c>
-      <c r="C7">
-        <v>2492</v>
-      </c>
-      <c r="D7">
-        <v>8127</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>3</v>
-      </c>
-      <c r="B8">
-        <v>12773</v>
-      </c>
-      <c r="C8">
-        <v>5990</v>
-      </c>
-      <c r="D8">
-        <v>18763</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>4</v>
-      </c>
-      <c r="B9">
-        <v>49718</v>
-      </c>
-      <c r="C9">
-        <v>15844</v>
-      </c>
-      <c r="D9">
-        <v>65562</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>5</v>
-      </c>
-      <c r="B10">
-        <v>4637</v>
-      </c>
-      <c r="C10">
-        <v>2036</v>
-      </c>
-      <c r="D10">
-        <v>6673</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>6</v>
-      </c>
-      <c r="B11">
-        <v>579</v>
-      </c>
-      <c r="C11">
-        <v>1071</v>
-      </c>
-      <c r="D11">
-        <v>1650</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>7</v>
-      </c>
-      <c r="B12">
-        <v>173</v>
-      </c>
-      <c r="C12">
-        <v>48</v>
-      </c>
-      <c r="D12">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>8</v>
-      </c>
-      <c r="B13">
-        <v>1842</v>
-      </c>
-      <c r="C13">
-        <v>1929</v>
-      </c>
-      <c r="D13">
-        <v>3771</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>9</v>
-      </c>
-      <c r="B14">
-        <v>2819</v>
-      </c>
-      <c r="C14">
-        <v>2388</v>
-      </c>
-      <c r="D14">
-        <v>5207</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>10</v>
-      </c>
-      <c r="B15">
-        <v>708</v>
-      </c>
-      <c r="C15">
-        <v>193</v>
-      </c>
-      <c r="D15">
-        <v>901</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>11</v>
-      </c>
-      <c r="B16">
-        <v>1358</v>
-      </c>
-      <c r="C16">
-        <v>1294</v>
-      </c>
-      <c r="D16">
-        <v>2652</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>12</v>
-      </c>
-      <c r="B17">
-        <v>1820</v>
-      </c>
-      <c r="C17">
-        <v>2570</v>
-      </c>
-      <c r="D17">
-        <v>4390</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>13</v>
-      </c>
-      <c r="B18">
-        <v>2284</v>
-      </c>
-      <c r="C18">
-        <v>2312</v>
-      </c>
-      <c r="D18">
-        <v>4596</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>14</v>
-      </c>
-      <c r="B19">
-        <v>1942</v>
-      </c>
-      <c r="C19">
-        <v>1079</v>
-      </c>
-      <c r="D19">
-        <v>3021</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>15</v>
-      </c>
-      <c r="B20">
-        <v>16975</v>
-      </c>
-      <c r="C20">
-        <v>13606</v>
-      </c>
-      <c r="D20">
-        <v>30581</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>16</v>
-      </c>
-      <c r="B21">
-        <v>4912</v>
-      </c>
-      <c r="C21">
-        <v>4412</v>
-      </c>
-      <c r="D21">
-        <v>9324</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>17</v>
-      </c>
-      <c r="B22">
-        <v>2562</v>
-      </c>
-      <c r="C22">
-        <v>1754</v>
-      </c>
-      <c r="D22">
-        <v>4316</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
-        <v>18</v>
-      </c>
-      <c r="B23">
-        <v>7817</v>
-      </c>
-      <c r="C23">
-        <v>3731</v>
-      </c>
-      <c r="D23">
-        <v>11548</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
-        <v>19</v>
-      </c>
-      <c r="B24">
-        <v>1032</v>
-      </c>
-      <c r="C24">
-        <v>465</v>
-      </c>
-      <c r="D24">
-        <v>1497</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
-        <v>20</v>
-      </c>
-      <c r="B25">
-        <v>1860</v>
-      </c>
-      <c r="C25">
-        <v>945</v>
-      </c>
-      <c r="D25">
-        <v>2805</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
-        <v>21</v>
-      </c>
-      <c r="B26">
-        <v>2270</v>
-      </c>
-      <c r="C26">
-        <v>756</v>
-      </c>
-      <c r="D26">
-        <v>3026</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
-        <v>22</v>
-      </c>
-      <c r="B27">
-        <v>4007</v>
-      </c>
-      <c r="C27">
-        <v>1945</v>
-      </c>
-      <c r="D27">
-        <v>5952</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
-        <v>23</v>
-      </c>
-      <c r="B28">
-        <v>1685</v>
-      </c>
-      <c r="C28">
-        <v>3530</v>
-      </c>
-      <c r="D28">
-        <v>5215</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
-        <v>24</v>
-      </c>
-      <c r="B29">
-        <v>3025</v>
-      </c>
-      <c r="C29">
-        <v>2825</v>
-      </c>
-      <c r="D29">
-        <v>5850</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
-        <v>25</v>
-      </c>
-      <c r="B30">
-        <v>1958</v>
-      </c>
-      <c r="C30">
-        <v>2556</v>
-      </c>
-      <c r="D30">
-        <v>4514</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
-        <v>26</v>
-      </c>
-      <c r="B32">
-        <v>156488</v>
-      </c>
-      <c r="C32">
-        <v>86353</v>
-      </c>
-      <c r="D32">
-        <v>242841</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>